<commit_message>
bab 5 on going
</commit_message>
<xml_diff>
--- a/2. Proposal/Metode/Try.xlsx
+++ b/2. Proposal/Metode/Try.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\File\Skripsi\2. Proposal\Metode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C36B71A-CB0F-4214-B570-50EA3EBB88B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90737B10-857C-4BC4-810B-0A112993BA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{9E0B27B6-5960-4ADA-83F0-0309D2A69620}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{9E0B27B6-5960-4ADA-83F0-0309D2A69620}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="Moving Average" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Moving Average" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="76">
   <si>
     <t>Tanggal</t>
   </si>
@@ -277,7 +278,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -357,6 +358,15 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -687,7 +697,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -887,6 +897,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7420,7 +7438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6B0E80-D10A-4815-A892-18FD744DDE32}">
   <dimension ref="B1:T95"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -9599,8 +9617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2841FB6-975F-477D-89A2-D948C0B29F1F}">
   <dimension ref="B1:W455"/>
   <sheetViews>
-    <sheetView topLeftCell="A100" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView topLeftCell="A102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T114" sqref="T114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25245,7 +25263,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2D8C26-AEFB-4D9E-9A41-28D820AB24F4}">
   <dimension ref="B1:N416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
+    <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="F3" sqref="F3:F32"/>
     </sheetView>
   </sheetViews>
@@ -31055,6 +31073,344 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A85AC635-D9F1-4122-B067-579C0A1EBE2C}">
+  <dimension ref="A1:M15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="95" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="95" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="78" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="94">
+        <v>1</v>
+      </c>
+      <c r="B2" s="94">
+        <v>6</v>
+      </c>
+      <c r="C2" s="93">
+        <f>A2^2</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="93">
+        <f>A2*B2</f>
+        <v>6</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="94">
+        <v>2</v>
+      </c>
+      <c r="B3" s="94">
+        <v>6</v>
+      </c>
+      <c r="C3" s="93">
+        <f t="shared" ref="C3:C15" si="0">A3^2</f>
+        <v>4</v>
+      </c>
+      <c r="D3" s="93">
+        <f t="shared" ref="D3:D15" si="1">A3*B3</f>
+        <v>12</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3">
+        <f>SUM(A2:A15)</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="94">
+        <v>3</v>
+      </c>
+      <c r="B4" s="94">
+        <v>18</v>
+      </c>
+      <c r="C4" s="93">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D4" s="93">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4">
+        <f>SUM(B2:B15)</f>
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="94">
+        <v>4</v>
+      </c>
+      <c r="B5" s="94">
+        <v>26</v>
+      </c>
+      <c r="C5" s="93">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D5" s="93">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5">
+        <f>SUM(C2:C15)</f>
+        <v>1015</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="94">
+        <v>5</v>
+      </c>
+      <c r="B6" s="94">
+        <v>23</v>
+      </c>
+      <c r="C6" s="93">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D6" s="93">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6">
+        <f>SUM(D2:D15)</f>
+        <v>2304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="94">
+        <v>6</v>
+      </c>
+      <c r="B7" s="94">
+        <v>11</v>
+      </c>
+      <c r="C7" s="93">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D7" s="93">
+        <f t="shared" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7">
+        <f>COUNT(A2:A15)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="94">
+        <v>7</v>
+      </c>
+      <c r="B8" s="94">
+        <v>12</v>
+      </c>
+      <c r="C8" s="93">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D8" s="93">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="94">
+        <v>8</v>
+      </c>
+      <c r="B9" s="94">
+        <v>24</v>
+      </c>
+      <c r="C9" s="93">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="D9" s="93">
+        <f t="shared" si="1"/>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="94">
+        <v>9</v>
+      </c>
+      <c r="B10" s="94">
+        <v>52</v>
+      </c>
+      <c r="C10" s="93">
+        <f t="shared" si="0"/>
+        <v>81</v>
+      </c>
+      <c r="D10" s="93">
+        <f t="shared" si="1"/>
+        <v>468</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10">
+        <f>((G4*G5)-(G3*G6))/((G7*G5)-(G3)^2)</f>
+        <v>12.637362637362637</v>
+      </c>
+      <c r="I10">
+        <f>INTERCEPT(B2:B15,A2:A15)</f>
+        <v>12.637362637362639</v>
+      </c>
+      <c r="K10">
+        <f>((G4*G5)-(G3*G6))</f>
+        <v>40250</v>
+      </c>
+      <c r="M10">
+        <f>((G7*G6)-(G3*G4))</f>
+        <v>3066</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="94">
+        <v>10</v>
+      </c>
+      <c r="B11" s="94">
+        <v>22</v>
+      </c>
+      <c r="C11" s="93">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="D11" s="93">
+        <f t="shared" si="1"/>
+        <v>220</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11">
+        <f>((G7*G6)-(G3*G4))/((G7*G5)-(G3)^2)</f>
+        <v>0.96263736263736266</v>
+      </c>
+      <c r="I11">
+        <f>SLOPE(B2:B15,A2:A15)</f>
+        <v>0.96263736263736255</v>
+      </c>
+      <c r="K11">
+        <f>((G7*G5)-(G3)^2)</f>
+        <v>3185</v>
+      </c>
+      <c r="M11">
+        <f>((G7*G5)-(G3)^2)</f>
+        <v>3185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="94">
+        <v>11</v>
+      </c>
+      <c r="B12" s="94">
+        <v>22</v>
+      </c>
+      <c r="C12" s="93">
+        <f t="shared" si="0"/>
+        <v>121</v>
+      </c>
+      <c r="D12" s="93">
+        <f t="shared" si="1"/>
+        <v>242</v>
+      </c>
+      <c r="K12" s="96">
+        <f>K10/K11</f>
+        <v>12.637362637362637</v>
+      </c>
+      <c r="M12" s="96">
+        <f>M10/M11</f>
+        <v>0.96263736263736266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="94">
+        <v>12</v>
+      </c>
+      <c r="B13" s="94">
+        <v>7</v>
+      </c>
+      <c r="C13" s="93">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="D13" s="93">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="94">
+        <v>13</v>
+      </c>
+      <c r="B14" s="94">
+        <v>29</v>
+      </c>
+      <c r="C14" s="93">
+        <f t="shared" si="0"/>
+        <v>169</v>
+      </c>
+      <c r="D14" s="93">
+        <f t="shared" si="1"/>
+        <v>377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="94">
+        <v>14</v>
+      </c>
+      <c r="B15" s="94">
+        <v>20</v>
+      </c>
+      <c r="C15" s="93">
+        <f t="shared" si="0"/>
+        <v>196</v>
+      </c>
+      <c r="D15" s="93">
+        <f t="shared" si="1"/>
+        <v>280</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B026BD2-121D-4666-92E5-527DA859B32C}">
   <dimension ref="A1:E446"/>
   <sheetViews>

</xml_diff>